<commit_message>
Correções no Código e na DataBase
</commit_message>
<xml_diff>
--- a/População Inicial - SI.xlsx
+++ b/População Inicial - SI.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="28785" windowHeight="12930"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Professores" sheetId="1" r:id="rId4"/>
+    <sheet name="Professores" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="8yBn414b7bxq8u0fXfDuSbOhbzVvn6IGna++/Pgep6o="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -30,7 +28,7 @@
     <t>Francisco Carlos Monteiro Souza</t>
   </si>
   <si>
-    <t>Segunda</t>
+    <t>01/12/2023;</t>
   </si>
   <si>
     <t>07:00-09:00;13:00-15:00</t>
@@ -39,13 +37,13 @@
     <t>Andre Roberto Ortoncelli</t>
   </si>
   <si>
-    <t>Terca;Quarta</t>
+    <t>02/12/2023;03/12/2023</t>
   </si>
   <si>
     <t>Lincoln Magalhães Costa</t>
   </si>
   <si>
-    <t>Quinta;Sexta</t>
+    <t>04/12/2023;05/12/2023</t>
   </si>
   <si>
     <t>Alinne Cristinne Correa Souza</t>
@@ -102,61 +100,916 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
+    <cellStyle name="Observação" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Saída" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
+    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Bom" xfId="22" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
+    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
+    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
+    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
+    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
+    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -346,26 +1199,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.88"/>
-    <col customWidth="1" min="2" max="2" width="17.13"/>
-    <col customWidth="1" min="3" max="3" width="22.5"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
+    <col min="1" max="1" width="27.8761904761905" customWidth="1"/>
+    <col min="2" max="2" width="22.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="22.5047619047619" customWidth="1"/>
+    <col min="4" max="6" width="12.6285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -376,18 +1233,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="15.75" customHeight="1" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -398,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -409,18 +1266,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15.75" customHeight="1" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -431,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -442,18 +1299,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="15.75" customHeight="1" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" ht="15.75" customHeight="1" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -464,7 +1321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" ht="15.75" customHeight="1" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -475,18 +1332,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" ht="15.75" customHeight="1" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" ht="15.75" customHeight="1" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -497,7 +1354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" ht="15.75" customHeight="1" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -508,18 +1365,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" ht="15.75" customHeight="1" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" ht="15.75" customHeight="1" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -530,7 +1387,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" ht="15.75" customHeight="1" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -541,29 +1398,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" ht="15.75" customHeight="1" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" ht="15.75" customHeight="1" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" ht="15.75" customHeight="1" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -574,607 +1431,607 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1" spans="1:1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1" spans="1:1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1" spans="1:1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1" spans="1:1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1" spans="1:1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1" spans="1:1">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" ht="15.75" customHeight="1" spans="1:1">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" ht="15.75" customHeight="1" spans="1:1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" ht="15.75" customHeight="1" spans="1:1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" ht="15.75" customHeight="1" spans="1:1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" ht="15.75" customHeight="1" spans="1:1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" ht="15.75" customHeight="1" spans="1:1">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="15.75" customHeight="1" spans="1:1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" ht="15.75" customHeight="1" spans="1:1">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" ht="15.75" customHeight="1" spans="1:1">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" ht="15.75" customHeight="1" spans="1:1">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" ht="15.75" customHeight="1" spans="1:1">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" ht="15.75" customHeight="1" spans="1:1">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" ht="15.75" customHeight="1" spans="1:1">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" ht="15.75" customHeight="1" spans="1:1">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" ht="15.75" customHeight="1" spans="1:1">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" ht="15.75" customHeight="1" spans="1:1">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
+    <row r="50" ht="15.75" customHeight="1" spans="1:1">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" ht="15.75" customHeight="1" spans="1:1">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" ht="15.75" customHeight="1" spans="1:1">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" ht="15.75" customHeight="1" spans="1:1">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" ht="15.75" customHeight="1" spans="1:1">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" ht="15.75" customHeight="1" spans="1:1">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" ht="15.75" customHeight="1" spans="1:1">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" ht="15.75" customHeight="1" spans="1:1">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" ht="15.75" customHeight="1" spans="1:1">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" ht="15.75" customHeight="1" spans="1:1">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" ht="15.75" customHeight="1" spans="1:1">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" ht="15.75" customHeight="1" spans="1:1">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" ht="15.75" customHeight="1" spans="1:1">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" ht="15.75" customHeight="1" spans="1:1">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" ht="15.75" customHeight="1" spans="1:1">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" ht="15.75" customHeight="1" spans="1:1">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" ht="15.75" customHeight="1" spans="1:1">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" ht="15.75" customHeight="1" spans="1:1">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" ht="15.75" customHeight="1" spans="1:1">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" ht="15.75" customHeight="1" spans="1:1">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" ht="15.75" customHeight="1" spans="1:1">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" ht="15.75" customHeight="1" spans="1:1">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" ht="15.75" customHeight="1" spans="1:1">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" ht="15.75" customHeight="1" spans="1:1">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" ht="15.75" customHeight="1" spans="1:1">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" ht="15.75" customHeight="1" spans="1:1">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
+    <row r="76" ht="15.75" customHeight="1" spans="1:1">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
+    <row r="77" ht="15.75" customHeight="1" spans="1:1">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
+    <row r="78" ht="15.75" customHeight="1" spans="1:1">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
+    <row r="79" ht="15.75" customHeight="1" spans="1:1">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
+    <row r="80" ht="15.75" customHeight="1" spans="1:1">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
+    <row r="81" ht="15.75" customHeight="1" spans="1:1">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
+    <row r="82" ht="15.75" customHeight="1" spans="1:1">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
+    <row r="83" ht="15.75" customHeight="1" spans="1:1">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
+    <row r="84" ht="15.75" customHeight="1" spans="1:1">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
+    <row r="85" ht="15.75" customHeight="1" spans="1:1">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
+    <row r="86" ht="15.75" customHeight="1" spans="1:1">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
+    <row r="87" ht="15.75" customHeight="1" spans="1:1">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
+    <row r="88" ht="15.75" customHeight="1" spans="1:1">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
+    <row r="89" ht="15.75" customHeight="1" spans="1:1">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
+    <row r="90" ht="15.75" customHeight="1" spans="1:1">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
+    <row r="91" ht="15.75" customHeight="1" spans="1:1">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
+    <row r="92" ht="15.75" customHeight="1" spans="1:1">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
+    <row r="93" ht="15.75" customHeight="1" spans="1:1">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
+    <row r="94" ht="15.75" customHeight="1" spans="1:1">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
+    <row r="95" ht="15.75" customHeight="1" spans="1:1">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
+    <row r="96" ht="15.75" customHeight="1" spans="1:1">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
+    <row r="97" ht="15.75" customHeight="1" spans="1:1">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1">
+    <row r="98" ht="15.75" customHeight="1" spans="1:1">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1">
+    <row r="99" ht="15.75" customHeight="1" spans="1:1">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1">
+    <row r="100" ht="15.75" customHeight="1" spans="1:1">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1">
+    <row r="101" ht="15.75" customHeight="1" spans="1:1">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1">
+    <row r="102" ht="15.75" customHeight="1" spans="1:1">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1">
+    <row r="103" ht="15.75" customHeight="1" spans="1:1">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1">
+    <row r="104" ht="15.75" customHeight="1" spans="1:1">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1">
+    <row r="105" ht="15.75" customHeight="1" spans="1:1">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1">
+    <row r="106" ht="15.75" customHeight="1" spans="1:1">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1">
+    <row r="107" ht="15.75" customHeight="1" spans="1:1">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1">
+    <row r="108" ht="15.75" customHeight="1" spans="1:1">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1">
+    <row r="109" ht="15.75" customHeight="1" spans="1:1">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1">
+    <row r="110" ht="15.75" customHeight="1" spans="1:1">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1">
+    <row r="111" ht="15.75" customHeight="1" spans="1:1">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1">
+    <row r="112" ht="15.75" customHeight="1" spans="1:1">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1">
+    <row r="113" ht="15.75" customHeight="1" spans="1:1">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1">
+    <row r="114" ht="15.75" customHeight="1" spans="1:1">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1">
+    <row r="115" ht="15.75" customHeight="1" spans="1:1">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1">
+    <row r="116" ht="15.75" customHeight="1" spans="1:1">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1">
+    <row r="117" ht="15.75" customHeight="1" spans="1:1">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1">
+    <row r="118" ht="15.75" customHeight="1" spans="1:1">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1">
+    <row r="119" ht="15.75" customHeight="1" spans="1:1">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1">
+    <row r="120" ht="15.75" customHeight="1" spans="1:1">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1">
+    <row r="121" ht="15.75" customHeight="1" spans="1:1">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1">
+    <row r="122" ht="15.75" customHeight="1" spans="1:1">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1">
+    <row r="123" ht="15.75" customHeight="1" spans="1:1">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1">
+    <row r="124" ht="15.75" customHeight="1" spans="1:1">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1">
+    <row r="125" ht="15.75" customHeight="1" spans="1:1">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1">
+    <row r="126" ht="15.75" customHeight="1" spans="1:1">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1">
+    <row r="127" ht="15.75" customHeight="1" spans="1:1">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1">
+    <row r="128" ht="15.75" customHeight="1" spans="1:1">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1">
+    <row r="129" ht="15.75" customHeight="1" spans="1:1">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1">
+    <row r="130" ht="15.75" customHeight="1" spans="1:1">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1">
+    <row r="131" ht="15.75" customHeight="1" spans="1:1">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1">
+    <row r="132" ht="15.75" customHeight="1" spans="1:1">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1">
+    <row r="133" ht="15.75" customHeight="1" spans="1:1">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1">
+    <row r="134" ht="15.75" customHeight="1" spans="1:1">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1">
+    <row r="135" ht="15.75" customHeight="1" spans="1:1">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1">
+    <row r="136" ht="15.75" customHeight="1" spans="1:1">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1">
+    <row r="137" ht="15.75" customHeight="1" spans="1:1">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1">
+    <row r="138" ht="15.75" customHeight="1" spans="1:1">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1">
+    <row r="139" ht="15.75" customHeight="1" spans="1:1">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1">
+    <row r="140" ht="15.75" customHeight="1" spans="1:1">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1">
+    <row r="141" ht="15.75" customHeight="1" spans="1:1">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
+    <row r="142" ht="15.75" customHeight="1" spans="1:1">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1">
+    <row r="143" ht="15.75" customHeight="1" spans="1:1">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1">
+    <row r="144" ht="15.75" customHeight="1" spans="1:1">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1">
+    <row r="145" ht="15.75" customHeight="1" spans="1:1">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1">
+    <row r="146" ht="15.75" customHeight="1" spans="1:1">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1">
+    <row r="147" ht="15.75" customHeight="1" spans="1:1">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1">
+    <row r="148" ht="15.75" customHeight="1" spans="1:1">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1">
+    <row r="149" ht="15.75" customHeight="1" spans="1:1">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1">
+    <row r="150" ht="15.75" customHeight="1" spans="1:1">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1">
+    <row r="151" ht="15.75" customHeight="1" spans="1:1">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1">
+    <row r="152" ht="15.75" customHeight="1" spans="1:1">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" ht="15.75" customHeight="1" spans="1:1">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1">
+    <row r="154" ht="15.75" customHeight="1" spans="1:1">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" ht="15.75" customHeight="1" spans="1:1">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" ht="15.75" customHeight="1" spans="1:1">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" ht="15.75" customHeight="1" spans="1:1">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1">
+    <row r="158" ht="15.75" customHeight="1" spans="1:1">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1">
+    <row r="159" ht="15.75" customHeight="1" spans="1:1">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1">
+    <row r="160" ht="15.75" customHeight="1" spans="1:1">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1">
+    <row r="161" ht="15.75" customHeight="1" spans="1:1">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1">
+    <row r="162" ht="15.75" customHeight="1" spans="1:1">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1">
+    <row r="163" ht="15.75" customHeight="1" spans="1:1">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1">
+    <row r="164" ht="15.75" customHeight="1" spans="1:1">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1">
+    <row r="165" ht="15.75" customHeight="1" spans="1:1">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1">
+    <row r="166" ht="15.75" customHeight="1" spans="1:1">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1">
+    <row r="167" ht="15.75" customHeight="1" spans="1:1">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1">
+    <row r="168" ht="15.75" customHeight="1" spans="1:1">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1">
+    <row r="169" ht="15.75" customHeight="1" spans="1:1">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1">
+    <row r="170" ht="15.75" customHeight="1" spans="1:1">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1">
+    <row r="171" ht="15.75" customHeight="1" spans="1:1">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1">
+    <row r="172" ht="15.75" customHeight="1" spans="1:1">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1">
+    <row r="173" ht="15.75" customHeight="1" spans="1:1">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1">
+    <row r="174" ht="15.75" customHeight="1" spans="1:1">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1">
+    <row r="175" ht="15.75" customHeight="1" spans="1:1">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1">
+    <row r="176" ht="15.75" customHeight="1" spans="1:1">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1">
+    <row r="177" ht="15.75" customHeight="1" spans="1:1">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1">
+    <row r="178" ht="15.75" customHeight="1" spans="1:1">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1">
+    <row r="179" ht="15.75" customHeight="1" spans="1:1">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1">
+    <row r="180" ht="15.75" customHeight="1" spans="1:1">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1">
+    <row r="181" ht="15.75" customHeight="1" spans="1:1">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1">
+    <row r="182" ht="15.75" customHeight="1" spans="1:1">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1">
+    <row r="183" ht="15.75" customHeight="1" spans="1:1">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1">
+    <row r="184" ht="15.75" customHeight="1" spans="1:1">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1">
+    <row r="185" ht="15.75" customHeight="1" spans="1:1">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1">
+    <row r="186" ht="15.75" customHeight="1" spans="1:1">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1">
+    <row r="187" ht="15.75" customHeight="1" spans="1:1">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1">
+    <row r="188" ht="15.75" customHeight="1" spans="1:1">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1">
+    <row r="189" ht="15.75" customHeight="1" spans="1:1">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1">
+    <row r="190" ht="15.75" customHeight="1" spans="1:1">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1">
+    <row r="191" ht="15.75" customHeight="1" spans="1:1">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1">
+    <row r="192" ht="15.75" customHeight="1" spans="1:1">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1">
+    <row r="193" ht="15.75" customHeight="1" spans="1:1">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1">
+    <row r="194" ht="15.75" customHeight="1" spans="1:1">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1">
+    <row r="195" ht="15.75" customHeight="1" spans="1:1">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1">
+    <row r="196" ht="15.75" customHeight="1" spans="1:1">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1">
+    <row r="197" ht="15.75" customHeight="1" spans="1:1">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1">
+    <row r="198" ht="15.75" customHeight="1" spans="1:1">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1">
+    <row r="199" ht="15.75" customHeight="1" spans="1:1">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" ht="15.75" customHeight="1" spans="1:1">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" ht="15.75" customHeight="1" spans="1:1">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" ht="15.75" customHeight="1" spans="1:1">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1">
+    <row r="203" ht="15.75" customHeight="1" spans="1:1">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" ht="15.75" customHeight="1" spans="1:1">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1">
+    <row r="205" ht="15.75" customHeight="1" spans="1:1">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" ht="15.75" customHeight="1" spans="1:1">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" ht="15.75" customHeight="1" spans="1:1">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1">
+    <row r="208" ht="15.75" customHeight="1" spans="1:1">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1">
+    <row r="209" ht="15.75" customHeight="1" spans="1:1">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" ht="15.75" customHeight="1" spans="1:1">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1">
+    <row r="211" ht="15.75" customHeight="1" spans="1:1">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1">
+    <row r="212" ht="15.75" customHeight="1" spans="1:1">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" ht="15.75" customHeight="1" spans="1:1">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" ht="15.75" customHeight="1" spans="1:1">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" ht="15.75" customHeight="1" spans="1:1">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1">
+    <row r="216" ht="15.75" customHeight="1" spans="1:1">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1">
+    <row r="217" ht="15.75" customHeight="1" spans="1:1">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1">
+    <row r="218" ht="15.75" customHeight="1" spans="1:1">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" ht="15.75" customHeight="1" spans="1:1">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1">
+    <row r="220" ht="15.75" customHeight="1" spans="1:1">
       <c r="A220" s="1"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
@@ -1958,6 +2815,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste na Planilha e no tamanho da população
</commit_message>
<xml_diff>
--- a/População Inicial - SI.xlsx
+++ b/População Inicial - SI.xlsx
@@ -1,15 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView windowWidth="28785" windowHeight="12930"/>
-  </bookViews>
   <sheets>
-    <sheet name="Professores" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Professores" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -25,7 +22,7 @@
     <t>Horario</t>
   </si>
   <si>
-    <t>Francisco Carlos Monteiro Souza</t>
+    <t>Fulano 1</t>
   </si>
   <si>
     <t>01/12/2023;</t>
@@ -34,982 +31,128 @@
     <t>07:00-09:00;13:00-15:00</t>
   </si>
   <si>
-    <t>Andre Roberto Ortoncelli</t>
+    <t>Fulano 2</t>
   </si>
   <si>
     <t>02/12/2023;03/12/2023</t>
   </si>
   <si>
-    <t>Lincoln Magalhães Costa</t>
+    <t>Fulano 3</t>
   </si>
   <si>
     <t>04/12/2023;05/12/2023</t>
   </si>
   <si>
-    <t>Alinne Cristinne Correa Souza</t>
-  </si>
-  <si>
-    <t>Rafael Alves Paes de Oliveira</t>
-  </si>
-  <si>
-    <t>Rodolfo Adamshuk Silva</t>
-  </si>
-  <si>
-    <t>Gustavo Jansen de Souza Santos</t>
+    <t>Fulano 4</t>
+  </si>
+  <si>
+    <t>Fulano 5</t>
+  </si>
+  <si>
+    <t>Fulano 6</t>
+  </si>
+  <si>
+    <t>Fulano 7</t>
   </si>
   <si>
     <t>09:00-11:00;15:00-17:00</t>
   </si>
   <si>
-    <t>Franciele Beal</t>
-  </si>
-  <si>
-    <t>Marisangela Pacheco Brittes</t>
-  </si>
-  <si>
-    <t>Newton Carlos Will</t>
-  </si>
-  <si>
-    <t>Simone de Sousa Borges</t>
-  </si>
-  <si>
-    <t>Evandro Miguel Kuszera</t>
-  </si>
-  <si>
-    <t>Tatianne Costa Negri Rocha</t>
+    <t>Fulano 8</t>
+  </si>
+  <si>
+    <t>Fulano 9</t>
+  </si>
+  <si>
+    <t>Fulano 10</t>
+  </si>
+  <si>
+    <t>Fulano 11</t>
+  </si>
+  <si>
+    <t>Fulano 12</t>
+  </si>
+  <si>
+    <t>Fulano 13</t>
   </si>
   <si>
     <t>17:00-19:00;19:00-21:00</t>
   </si>
   <si>
-    <t>Maria Adelina Silva Brito</t>
-  </si>
-  <si>
-    <t>Rene Pomilio de Oliveira</t>
-  </si>
-  <si>
-    <t>Paula Fernandes Montanher</t>
-  </si>
-  <si>
-    <t>Maristela Dos Santos Rey</t>
-  </si>
-  <si>
-    <t>Ricardo Ferreira Vilela</t>
+    <t>Fulano 14</t>
+  </si>
+  <si>
+    <t>Fulano 15</t>
+  </si>
+  <si>
+    <t>Fulano 16</t>
+  </si>
+  <si>
+    <t>Fulano 17</t>
+  </si>
+  <si>
+    <t>Fulano 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="9">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
-    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
-    <cellStyle name="Observação" xfId="8" builtinId="10"/>
-    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
-    <cellStyle name="Título" xfId="10" builtinId="15"/>
-    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
-    <cellStyle name="Saída" xfId="17" builtinId="21"/>
-    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
-    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
-    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Bom" xfId="22" builtinId="26"/>
-    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
-    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
-    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
-    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
-    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
-    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
-    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
-    </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
-    </tableStyle>
-  </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1199,30 +342,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.8761904761905" customWidth="1"/>
-    <col min="2" max="2" width="22.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="22.5047619047619" customWidth="1"/>
-    <col min="4" max="6" width="12.6285714285714" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="27.88"/>
+    <col customWidth="1" min="2" max="2" width="22.63"/>
+    <col customWidth="1" min="3" max="3" width="22.5"/>
+    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:3">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1233,19 +373,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1255,8 +395,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1266,19 +406,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1288,8 +428,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1299,19 +439,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1321,8 +461,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A10" s="1" t="s">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1332,19 +472,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A11" s="1" t="s">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A12" s="1" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1354,8 +494,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A13" s="1" t="s">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1365,19 +505,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A15" s="1" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1387,8 +527,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1398,30 +538,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A17" s="1" t="s">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A19" s="1" t="s">
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1431,607 +571,607 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" spans="1:1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:1">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1" spans="1:1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1" spans="1:1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1" spans="1:1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1" spans="1:1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1" spans="1:1">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1" spans="1:1">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1" spans="1:1">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1" spans="1:1">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1" spans="1:1">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1" spans="1:1">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" spans="1:1">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1" spans="1:1">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1" spans="1:1">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1" spans="1:1">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1" spans="1:1">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1" spans="1:1">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1" spans="1:1">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1" spans="1:1">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1" spans="1:1">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1" spans="1:1">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1" spans="1:1">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1" spans="1:1">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1" spans="1:1">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1" spans="1:1">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1" spans="1:1">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1" spans="1:1">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1" spans="1:1">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1" spans="1:1">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1" spans="1:1">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1" spans="1:1">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1" spans="1:1">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1" spans="1:1">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1" spans="1:1">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1" spans="1:1">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1" spans="1:1">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1" spans="1:1">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1" spans="1:1">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1" spans="1:1">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1" spans="1:1">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1" spans="1:1">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1" spans="1:1">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1" spans="1:1">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1" spans="1:1">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1" spans="1:1">
+    <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1" spans="1:1">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1" spans="1:1">
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1" spans="1:1">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1" spans="1:1">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1" spans="1:1">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1" spans="1:1">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1" spans="1:1">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1" spans="1:1">
+    <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1" spans="1:1">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1" spans="1:1">
+    <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1" spans="1:1">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1" spans="1:1">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1" spans="1:1">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1" spans="1:1">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1" spans="1:1">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1" spans="1:1">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1" spans="1:1">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1" spans="1:1">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1" spans="1:1">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1" spans="1:1">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1" spans="1:1">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1" spans="1:1">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1" spans="1:1">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1" spans="1:1">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1" spans="1:1">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" ht="15.75" customHeight="1" spans="1:1">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" ht="15.75" customHeight="1" spans="1:1">
+    <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" ht="15.75" customHeight="1" spans="1:1">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" ht="15.75" customHeight="1" spans="1:1">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1" spans="1:1">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" ht="15.75" customHeight="1" spans="1:1">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" ht="15.75" customHeight="1" spans="1:1">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" ht="15.75" customHeight="1" spans="1:1">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1" spans="1:1">
+    <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" ht="15.75" customHeight="1" spans="1:1">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" ht="15.75" customHeight="1" spans="1:1">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" ht="15.75" customHeight="1" spans="1:1">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" ht="15.75" customHeight="1" spans="1:1">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" ht="15.75" customHeight="1" spans="1:1">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" ht="15.75" customHeight="1" spans="1:1">
+    <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" ht="15.75" customHeight="1" spans="1:1">
+    <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" ht="15.75" customHeight="1" spans="1:1">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" ht="15.75" customHeight="1" spans="1:1">
+    <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" ht="15.75" customHeight="1" spans="1:1">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" ht="15.75" customHeight="1" spans="1:1">
+    <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" ht="15.75" customHeight="1" spans="1:1">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" ht="15.75" customHeight="1" spans="1:1">
+    <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" ht="15.75" customHeight="1" spans="1:1">
+    <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" ht="15.75" customHeight="1" spans="1:1">
+    <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" ht="15.75" customHeight="1" spans="1:1">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" ht="15.75" customHeight="1" spans="1:1">
+    <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" ht="15.75" customHeight="1" spans="1:1">
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" ht="15.75" customHeight="1" spans="1:1">
+    <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" ht="15.75" customHeight="1" spans="1:1">
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" ht="15.75" customHeight="1" spans="1:1">
+    <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" ht="15.75" customHeight="1" spans="1:1">
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" ht="15.75" customHeight="1" spans="1:1">
+    <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" ht="15.75" customHeight="1" spans="1:1">
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" ht="15.75" customHeight="1" spans="1:1">
+    <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" ht="15.75" customHeight="1" spans="1:1">
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" ht="15.75" customHeight="1" spans="1:1">
+    <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" ht="15.75" customHeight="1" spans="1:1">
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" ht="15.75" customHeight="1" spans="1:1">
+    <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" ht="15.75" customHeight="1" spans="1:1">
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" ht="15.75" customHeight="1" spans="1:1">
+    <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" ht="15.75" customHeight="1" spans="1:1">
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" ht="15.75" customHeight="1" spans="1:1">
+    <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" ht="15.75" customHeight="1" spans="1:1">
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" ht="15.75" customHeight="1" spans="1:1">
+    <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" ht="15.75" customHeight="1" spans="1:1">
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" ht="15.75" customHeight="1" spans="1:1">
+    <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" ht="15.75" customHeight="1" spans="1:1">
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" ht="15.75" customHeight="1" spans="1:1">
+    <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" ht="15.75" customHeight="1" spans="1:1">
+    <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" ht="15.75" customHeight="1" spans="1:1">
+    <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" ht="15.75" customHeight="1" spans="1:1">
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" ht="15.75" customHeight="1" spans="1:1">
+    <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" ht="15.75" customHeight="1" spans="1:1">
+    <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" ht="15.75" customHeight="1" spans="1:1">
+    <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1" spans="1:1">
+    <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1" spans="1:1">
+    <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" ht="15.75" customHeight="1" spans="1:1">
+    <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1" spans="1:1">
+    <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1" spans="1:1">
+    <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1" spans="1:1">
+    <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" ht="15.75" customHeight="1" spans="1:1">
+    <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" ht="15.75" customHeight="1" spans="1:1">
+    <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" ht="15.75" customHeight="1" spans="1:1">
+    <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" ht="15.75" customHeight="1" spans="1:1">
+    <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" ht="15.75" customHeight="1" spans="1:1">
+    <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" ht="15.75" customHeight="1" spans="1:1">
+    <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" ht="15.75" customHeight="1" spans="1:1">
+    <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" ht="15.75" customHeight="1" spans="1:1">
+    <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" ht="15.75" customHeight="1" spans="1:1">
+    <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" ht="15.75" customHeight="1" spans="1:1">
+    <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" ht="15.75" customHeight="1" spans="1:1">
+    <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" ht="15.75" customHeight="1" spans="1:1">
+    <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" ht="15.75" customHeight="1" spans="1:1">
+    <row r="170" ht="15.75" customHeight="1">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" ht="15.75" customHeight="1" spans="1:1">
+    <row r="171" ht="15.75" customHeight="1">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" ht="15.75" customHeight="1" spans="1:1">
+    <row r="172" ht="15.75" customHeight="1">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" ht="15.75" customHeight="1" spans="1:1">
+    <row r="173" ht="15.75" customHeight="1">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" ht="15.75" customHeight="1" spans="1:1">
+    <row r="174" ht="15.75" customHeight="1">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" ht="15.75" customHeight="1" spans="1:1">
+    <row r="175" ht="15.75" customHeight="1">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" ht="15.75" customHeight="1" spans="1:1">
+    <row r="176" ht="15.75" customHeight="1">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" ht="15.75" customHeight="1" spans="1:1">
+    <row r="177" ht="15.75" customHeight="1">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" ht="15.75" customHeight="1" spans="1:1">
+    <row r="178" ht="15.75" customHeight="1">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" ht="15.75" customHeight="1" spans="1:1">
+    <row r="179" ht="15.75" customHeight="1">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" ht="15.75" customHeight="1" spans="1:1">
+    <row r="180" ht="15.75" customHeight="1">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" ht="15.75" customHeight="1" spans="1:1">
+    <row r="181" ht="15.75" customHeight="1">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" ht="15.75" customHeight="1" spans="1:1">
+    <row r="182" ht="15.75" customHeight="1">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" ht="15.75" customHeight="1" spans="1:1">
+    <row r="183" ht="15.75" customHeight="1">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" ht="15.75" customHeight="1" spans="1:1">
+    <row r="184" ht="15.75" customHeight="1">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" ht="15.75" customHeight="1" spans="1:1">
+    <row r="185" ht="15.75" customHeight="1">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" ht="15.75" customHeight="1" spans="1:1">
+    <row r="186" ht="15.75" customHeight="1">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" ht="15.75" customHeight="1" spans="1:1">
+    <row r="187" ht="15.75" customHeight="1">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" ht="15.75" customHeight="1" spans="1:1">
+    <row r="188" ht="15.75" customHeight="1">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" ht="15.75" customHeight="1" spans="1:1">
+    <row r="189" ht="15.75" customHeight="1">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" ht="15.75" customHeight="1" spans="1:1">
+    <row r="190" ht="15.75" customHeight="1">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" ht="15.75" customHeight="1" spans="1:1">
+    <row r="191" ht="15.75" customHeight="1">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" ht="15.75" customHeight="1" spans="1:1">
+    <row r="192" ht="15.75" customHeight="1">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" ht="15.75" customHeight="1" spans="1:1">
+    <row r="193" ht="15.75" customHeight="1">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" ht="15.75" customHeight="1" spans="1:1">
+    <row r="194" ht="15.75" customHeight="1">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" ht="15.75" customHeight="1" spans="1:1">
+    <row r="195" ht="15.75" customHeight="1">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" ht="15.75" customHeight="1" spans="1:1">
+    <row r="196" ht="15.75" customHeight="1">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" ht="15.75" customHeight="1" spans="1:1">
+    <row r="197" ht="15.75" customHeight="1">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" ht="15.75" customHeight="1" spans="1:1">
+    <row r="198" ht="15.75" customHeight="1">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" ht="15.75" customHeight="1" spans="1:1">
+    <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" ht="15.75" customHeight="1" spans="1:1">
+    <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" ht="15.75" customHeight="1" spans="1:1">
+    <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" ht="15.75" customHeight="1" spans="1:1">
+    <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" ht="15.75" customHeight="1" spans="1:1">
+    <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" ht="15.75" customHeight="1" spans="1:1">
+    <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" ht="15.75" customHeight="1" spans="1:1">
+    <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" ht="15.75" customHeight="1" spans="1:1">
+    <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" ht="15.75" customHeight="1" spans="1:1">
+    <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" ht="15.75" customHeight="1" spans="1:1">
+    <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1" spans="1:1">
+    <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" ht="15.75" customHeight="1" spans="1:1">
+    <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" ht="15.75" customHeight="1" spans="1:1">
+    <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" ht="15.75" customHeight="1" spans="1:1">
+    <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" ht="15.75" customHeight="1" spans="1:1">
+    <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" ht="15.75" customHeight="1" spans="1:1">
+    <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" ht="15.75" customHeight="1" spans="1:1">
+    <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1" spans="1:1">
+    <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1" spans="1:1">
+    <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1" spans="1:1">
+    <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1" spans="1:1">
+    <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1" spans="1:1">
+    <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="1"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
@@ -2815,7 +1955,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>